<commit_message>
- Tested the current setup with all the map. It works but the avoid policy cascade doesn't wotk really well still
</commit_message>
<xml_diff>
--- a/src/output/opt/all/data.xlsx
+++ b/src/output/opt/all/data.xlsx
@@ -53,24 +53,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3" customWidth="true"/>
-    <col min="2" max="2" width="5" customWidth="true"/>
-    <col min="3" max="3" width="2" customWidth="true"/>
-    <col min="4" max="4" width="3.5546875" customWidth="true"/>
-    <col min="5" max="5" width="4" customWidth="true"/>
-    <col min="6" max="6" width="4.5546875" customWidth="true"/>
-    <col min="7" max="7" width="4" customWidth="true"/>
-    <col min="8" max="8" width="11.5546875" customWidth="true"/>
-    <col min="9" max="9" width="15.5546875" customWidth="true"/>
-    <col min="10" max="10" width="15.88671875" customWidth="true"/>
-    <col min="11" max="11" width="2" customWidth="true"/>
-    <col min="12" max="12" width="3" customWidth="true"/>
+    <col min="1" max="1" width="3.140625" customWidth="true"/>
+    <col min="2" max="2" width="5.140625" customWidth="true"/>
+    <col min="3" max="3" width="2.140625" customWidth="true"/>
+    <col min="4" max="4" width="3.7109375" customWidth="true"/>
+    <col min="5" max="5" width="4.140625" customWidth="true"/>
+    <col min="6" max="6" width="4.7109375" customWidth="true"/>
+    <col min="7" max="7" width="4.140625" customWidth="true"/>
+    <col min="8" max="8" width="11.7109375" customWidth="true"/>
+    <col min="9" max="9" width="15.7109375" customWidth="true"/>
+    <col min="10" max="10" width="16.28515625" customWidth="true"/>
+    <col min="11" max="11" width="2.140625" customWidth="true"/>
+    <col min="12" max="12" width="3.140625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -96,13 +96,13 @@
         <v>233</v>
       </c>
       <c r="H1" s="0">
-        <v>26.040633100000001</v>
+        <v>30.8169106</v>
       </c>
       <c r="I1" s="0">
-        <v>0.0011669095536990248</v>
+        <v>0.0019058552724922073</v>
       </c>
       <c r="J1" s="0">
-        <v>6.1554448236762822e-06</v>
+        <v>1.8392708652162348e-05</v>
       </c>
       <c r="K1" s="0">
         <v>0</v>
@@ -131,22 +131,22 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G2" s="0">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="H2" s="0">
-        <v>82.178674900000004</v>
+        <v>81.300640999999999</v>
       </c>
       <c r="I2" s="0">
-        <v>0.00056683237757515492</v>
+        <v>0.0011763871526619951</v>
       </c>
       <c r="J2" s="0">
-        <v>5.2801134730241207e-06</v>
+        <v>1.3793771315107617e-05</v>
       </c>
       <c r="K2" s="0">
         <v>1</v>
       </c>
       <c r="L2" s="0">
-        <v>69</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
@@ -172,13 +172,13 @@
         <v>185</v>
       </c>
       <c r="H3" s="0">
-        <v>69.398217799999998</v>
+        <v>75.637316600000005</v>
       </c>
       <c r="I3" s="0">
-        <v>0.00056683237757515492</v>
+        <v>0.0011763871526619951</v>
       </c>
       <c r="J3" s="0">
-        <v>5.7302354582635842e-06</v>
+        <v>1.3561149916247957e-05</v>
       </c>
       <c r="K3" s="0">
         <v>0</v>
@@ -207,16 +207,16 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G4" s="0">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H4" s="0">
-        <v>109.9049476</v>
+        <v>165.3663291</v>
       </c>
       <c r="I4" s="0">
-        <v>0.00056683237757515492</v>
+        <v>0.0011763871526619951</v>
       </c>
       <c r="J4" s="0">
-        <v>5.8680983340737807e-06</v>
+        <v>1.3957391818017622e-05</v>
       </c>
       <c r="K4" s="0">
         <v>0</v>
@@ -248,19 +248,19 @@
         <v>163</v>
       </c>
       <c r="H5" s="0">
-        <v>70.378374800000003</v>
+        <v>85.326888999999994</v>
       </c>
       <c r="I5" s="0">
-        <v>0.00087689416471925519</v>
+        <v>0.0013907086057423079</v>
       </c>
       <c r="J5" s="0">
-        <v>6.2494118149673605e-06</v>
+        <v>2.0304716180701956e-05</v>
       </c>
       <c r="K5" s="0">
         <v>1</v>
       </c>
       <c r="L5" s="0">
-        <v>56</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
@@ -283,16 +283,16 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G6" s="0">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="H6" s="0">
-        <v>261.76413789999998</v>
+        <v>257.6468557</v>
       </c>
       <c r="I6" s="0">
-        <v>0.0013549857908126128</v>
+        <v>0.0024080313284957633</v>
       </c>
       <c r="J6" s="0">
-        <v>3.9018740795627191e-06</v>
+        <v>1.3723826764045608e-05</v>
       </c>
       <c r="K6" s="0">
         <v>0</v>
@@ -321,22 +321,22 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G7" s="0">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="H7" s="0">
-        <v>256.95693679999999</v>
+        <v>204.96942129999999</v>
       </c>
       <c r="I7" s="0">
-        <v>0.0013858646742737069</v>
+        <v>0.0029469436681917038</v>
       </c>
       <c r="J7" s="0">
-        <v>3.8131604398338645e-06</v>
+        <v>1.6598221994684326e-05</v>
       </c>
       <c r="K7" s="0">
         <v>1</v>
       </c>
       <c r="L7" s="0">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -359,22 +359,22 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G8" s="0">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H8" s="0">
-        <v>58.768913900000001</v>
+        <v>63.420286900000001</v>
       </c>
       <c r="I8" s="0">
-        <v>0.00045802723616250596</v>
+        <v>0.00032603169971578971</v>
       </c>
       <c r="J8" s="0">
-        <v>2.0602678764895812e-06</v>
+        <v>-2.7236118733130056e-06</v>
       </c>
       <c r="K8" s="0">
         <v>1</v>
       </c>
       <c r="L8" s="0">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9">
@@ -397,22 +397,22 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G9" s="0">
-        <v>228</v>
+        <v>165</v>
       </c>
       <c r="H9" s="0">
-        <v>135.1013888</v>
+        <v>94.326618999999994</v>
       </c>
       <c r="I9" s="0">
-        <v>0.1849463209999529</v>
+        <v>0.0072346880459221996</v>
       </c>
       <c r="J9" s="0">
-        <v>0.003189359716966217</v>
+        <v>4.4418400528355207e-05</v>
       </c>
       <c r="K9" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L9" s="0">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10">
@@ -435,22 +435,22 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G10" s="0">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="H10" s="0">
-        <v>107.69261179999999</v>
+        <v>146.1809193</v>
       </c>
       <c r="I10" s="0">
-        <v>0.0039184320439888953</v>
+        <v>0.00037825261720558778</v>
       </c>
       <c r="J10" s="0">
-        <v>-5.5182354747400761e-05</v>
+        <v>-2.7389651869448497e-05</v>
       </c>
       <c r="K10" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L10" s="0">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11">
@@ -473,16 +473,16 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G11" s="0">
-        <v>150</v>
+        <v>204</v>
       </c>
       <c r="H11" s="0">
-        <v>28.506793900000002</v>
+        <v>115.3778066</v>
       </c>
       <c r="I11" s="0">
-        <v>0.00087689416471925519</v>
+        <v>0.00090273012002684005</v>
       </c>
       <c r="J11" s="0">
-        <v>6.6248342670542173e-06</v>
+        <v>1.3570447126830444e-05</v>
       </c>
       <c r="K11" s="0">
         <v>0</v>
@@ -511,22 +511,22 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G12" s="0">
-        <v>153</v>
+        <v>180</v>
       </c>
       <c r="H12" s="0">
-        <v>68.576985300000004</v>
+        <v>116.0721434</v>
       </c>
       <c r="I12" s="0">
-        <v>0.00087689416471925519</v>
+        <v>0.0015245993471555419</v>
       </c>
       <c r="J12" s="0">
-        <v>6.8473717646703405e-06</v>
+        <v>-2.8272627787815734e-05</v>
       </c>
       <c r="K12" s="0">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L12" s="0">
-        <v>0</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13">
@@ -549,22 +549,22 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G13" s="0">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="H13" s="0">
-        <v>115.08578110000001</v>
+        <v>116.3119104</v>
       </c>
       <c r="I13" s="0">
-        <v>0.00054238354934654787</v>
+        <v>0.0019422957481607384</v>
       </c>
       <c r="J13" s="0">
-        <v>5.806515083048723e-06</v>
+        <v>-1.2999783357839103e-05</v>
       </c>
       <c r="K13" s="0">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L13" s="0">
-        <v>0</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14">
@@ -587,22 +587,136 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G14" s="0">
-        <v>346</v>
+        <v>150</v>
       </c>
       <c r="H14" s="0">
-        <v>179.96711450000001</v>
+        <v>27.7283103</v>
       </c>
       <c r="I14" s="0">
-        <v>0.029904831637027396</v>
+        <v>0.0013907086057423079</v>
       </c>
       <c r="J14" s="0">
-        <v>-3.3078495195644412e-06</v>
+        <v>1.9944768976384678e-05</v>
       </c>
       <c r="K14" s="0">
+        <v>0</v>
+      </c>
+      <c r="L14" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>10</v>
+      </c>
+      <c r="B15" s="0">
+        <v>1000</v>
+      </c>
+      <c r="C15" s="0">
+        <v>5</v>
+      </c>
+      <c r="D15" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="E15" s="0">
+        <v>100</v>
+      </c>
+      <c r="F15" s="0">
+        <v>0.94999999999999996</v>
+      </c>
+      <c r="G15" s="0">
+        <v>153</v>
+      </c>
+      <c r="H15" s="0">
+        <v>64.405401299999994</v>
+      </c>
+      <c r="I15" s="0">
+        <v>0.0013907086057423079</v>
+      </c>
+      <c r="J15" s="0">
+        <v>2.0256190713535646e-05</v>
+      </c>
+      <c r="K15" s="0">
+        <v>0</v>
+      </c>
+      <c r="L15" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>10</v>
+      </c>
+      <c r="B16" s="0">
+        <v>1000</v>
+      </c>
+      <c r="C16" s="0">
+        <v>5</v>
+      </c>
+      <c r="D16" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="E16" s="0">
+        <v>100</v>
+      </c>
+      <c r="F16" s="0">
+        <v>0.94999999999999996</v>
+      </c>
+      <c r="G16" s="0">
+        <v>165</v>
+      </c>
+      <c r="H16" s="0">
+        <v>94.311742300000006</v>
+      </c>
+      <c r="I16" s="0">
+        <v>0.0011907021309742749</v>
+      </c>
+      <c r="J16" s="0">
+        <v>1.5755517712114045e-05</v>
+      </c>
+      <c r="K16" s="0">
+        <v>0</v>
+      </c>
+      <c r="L16" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>10</v>
+      </c>
+      <c r="B17" s="0">
+        <v>1000</v>
+      </c>
+      <c r="C17" s="0">
+        <v>5</v>
+      </c>
+      <c r="D17" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="E17" s="0">
+        <v>100</v>
+      </c>
+      <c r="F17" s="0">
+        <v>0.94999999999999996</v>
+      </c>
+      <c r="G17" s="0">
+        <v>182</v>
+      </c>
+      <c r="H17" s="0">
+        <v>71.535492099999999</v>
+      </c>
+      <c r="I17" s="0">
+        <v>0.0023318558688201207</v>
+      </c>
+      <c r="J17" s="0">
+        <v>-7.3498151964727416e-05</v>
+      </c>
+      <c r="K17" s="0">
         <v>1</v>
       </c>
-      <c r="L14" s="0">
-        <v>170</v>
+      <c r="L17" s="0">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Tested the navigation policy cascade and works. - lab evironment doesnt work. - All the test work with good errors.
</commit_message>
<xml_diff>
--- a/src/output/opt/all/data.xlsx
+++ b/src/output/opt/all/data.xlsx
@@ -65,12 +65,12 @@
     <col min="4" max="4" width="3.7109375" customWidth="true"/>
     <col min="5" max="5" width="4.140625" customWidth="true"/>
     <col min="6" max="6" width="4.7109375" customWidth="true"/>
-    <col min="7" max="7" width="4.140625" customWidth="true"/>
+    <col min="7" max="7" width="5.140625" customWidth="true"/>
     <col min="8" max="8" width="11.7109375" customWidth="true"/>
     <col min="9" max="9" width="15.7109375" customWidth="true"/>
     <col min="10" max="10" width="16.28515625" customWidth="true"/>
     <col min="11" max="11" width="2.140625" customWidth="true"/>
-    <col min="12" max="12" width="3.140625" customWidth="true"/>
+    <col min="12" max="12" width="4.140625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -93,16 +93,16 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G1" s="0">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="H1" s="0">
-        <v>30.8169106</v>
+        <v>26.866167099999998</v>
       </c>
       <c r="I1" s="0">
-        <v>0.0019058552724922073</v>
+        <v>6.1648708908013106e-05</v>
       </c>
       <c r="J1" s="0">
-        <v>1.8392708652162348e-05</v>
+        <v>7.6485959938137463e-07</v>
       </c>
       <c r="K1" s="0">
         <v>0</v>
@@ -131,22 +131,22 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G2" s="0">
-        <v>200</v>
+        <v>269</v>
       </c>
       <c r="H2" s="0">
-        <v>81.300640999999999</v>
+        <v>73.478886000000003</v>
       </c>
       <c r="I2" s="0">
-        <v>0.0011763871526619951</v>
+        <v>6.5519894709487048e-05</v>
       </c>
       <c r="J2" s="0">
-        <v>1.3793771315107617e-05</v>
+        <v>5.0572873784854949e-07</v>
       </c>
       <c r="K2" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" s="0">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -169,16 +169,16 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G3" s="0">
-        <v>185</v>
+        <v>269</v>
       </c>
       <c r="H3" s="0">
-        <v>75.637316600000005</v>
+        <v>82.138268400000001</v>
       </c>
       <c r="I3" s="0">
-        <v>0.0011763871526619951</v>
+        <v>6.676530033189465e-05</v>
       </c>
       <c r="J3" s="0">
-        <v>1.3561149916247957e-05</v>
+        <v>5.1701806504116313e-07</v>
       </c>
       <c r="K3" s="0">
         <v>0</v>
@@ -207,16 +207,16 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G4" s="0">
-        <v>186</v>
+        <v>275</v>
       </c>
       <c r="H4" s="0">
-        <v>165.3663291</v>
+        <v>143.17481069999999</v>
       </c>
       <c r="I4" s="0">
-        <v>0.0011763871526619951</v>
+        <v>6.0603882801713027e-05</v>
       </c>
       <c r="J4" s="0">
-        <v>1.3957391818017622e-05</v>
+        <v>6.556261854759074e-07</v>
       </c>
       <c r="K4" s="0">
         <v>0</v>
@@ -245,22 +245,22 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G5" s="0">
-        <v>163</v>
+        <v>238</v>
       </c>
       <c r="H5" s="0">
-        <v>85.326888999999994</v>
+        <v>79.355134800000002</v>
       </c>
       <c r="I5" s="0">
-        <v>0.0013907086057423079</v>
+        <v>6.7715886985730833e-05</v>
       </c>
       <c r="J5" s="0">
-        <v>2.0304716180701956e-05</v>
+        <v>6.1785031100708851e-07</v>
       </c>
       <c r="K5" s="0">
         <v>1</v>
       </c>
       <c r="L5" s="0">
-        <v>25</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6">
@@ -283,16 +283,16 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G6" s="0">
-        <v>428</v>
+        <v>779</v>
       </c>
       <c r="H6" s="0">
-        <v>257.6468557</v>
+        <v>404.45322729999998</v>
       </c>
       <c r="I6" s="0">
-        <v>0.0024080313284957633</v>
+        <v>6.5152039799398764e-05</v>
       </c>
       <c r="J6" s="0">
-        <v>1.3723826764045608e-05</v>
+        <v>1.8010085309868908e-07</v>
       </c>
       <c r="K6" s="0">
         <v>0</v>
@@ -321,22 +321,22 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G7" s="0">
-        <v>487</v>
+        <v>1262</v>
       </c>
       <c r="H7" s="0">
-        <v>204.96942129999999</v>
+        <v>280.97373010000001</v>
       </c>
       <c r="I7" s="0">
-        <v>0.0029469436681917038</v>
+        <v>0.00015597136462863759</v>
       </c>
       <c r="J7" s="0">
-        <v>1.6598221994684326e-05</v>
+        <v>-1.6441482591255901e-06</v>
       </c>
       <c r="K7" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" s="0">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -359,22 +359,22 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G8" s="0">
-        <v>116</v>
+        <v>285</v>
       </c>
       <c r="H8" s="0">
-        <v>63.420286900000001</v>
+        <v>87.028548000000001</v>
       </c>
       <c r="I8" s="0">
-        <v>0.00032603169971578971</v>
+        <v>6.7987289118054406e-05</v>
       </c>
       <c r="J8" s="0">
-        <v>-2.7236118733130056e-06</v>
+        <v>4.3367886949577921e-07</v>
       </c>
       <c r="K8" s="0">
         <v>1</v>
       </c>
       <c r="L8" s="0">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9">
@@ -397,22 +397,22 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G9" s="0">
-        <v>165</v>
+        <v>312</v>
       </c>
       <c r="H9" s="0">
-        <v>94.326618999999994</v>
+        <v>94.783641700000004</v>
       </c>
       <c r="I9" s="0">
-        <v>0.0072346880459221996</v>
+        <v>6.8116042360788498e-05</v>
       </c>
       <c r="J9" s="0">
-        <v>4.4418400528355207e-05</v>
+        <v>6.0693372676457197e-07</v>
       </c>
       <c r="K9" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L9" s="0">
-        <v>48</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10">
@@ -435,22 +435,22 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G10" s="0">
-        <v>179</v>
+        <v>369</v>
       </c>
       <c r="H10" s="0">
-        <v>146.1809193</v>
+        <v>176.25475739999999</v>
       </c>
       <c r="I10" s="0">
-        <v>0.00037825261720558778</v>
+        <v>0.00018531213506078892</v>
       </c>
       <c r="J10" s="0">
-        <v>-2.7389651869448497e-05</v>
+        <v>-4.3988692627432443e-06</v>
       </c>
       <c r="K10" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L10" s="0">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11">
@@ -473,22 +473,22 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G11" s="0">
-        <v>204</v>
+        <v>269</v>
       </c>
       <c r="H11" s="0">
-        <v>115.3778066</v>
+        <v>161.8426977</v>
       </c>
       <c r="I11" s="0">
-        <v>0.00090273012002684005</v>
+        <v>0.00078415626376182601</v>
       </c>
       <c r="J11" s="0">
-        <v>1.3570447126830444e-05</v>
+        <v>-3.0608607912803039e-05</v>
       </c>
       <c r="K11" s="0">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L11" s="0">
-        <v>0</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12">
@@ -511,22 +511,22 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G12" s="0">
-        <v>180</v>
+        <v>269</v>
       </c>
       <c r="H12" s="0">
-        <v>116.0721434</v>
+        <v>243.20405769999999</v>
       </c>
       <c r="I12" s="0">
-        <v>0.0015245993471555419</v>
+        <v>0.00035683199620062389</v>
       </c>
       <c r="J12" s="0">
-        <v>-2.8272627787815734e-05</v>
+        <v>-3.9766926691228031e-05</v>
       </c>
       <c r="K12" s="0">
         <v>2</v>
       </c>
       <c r="L12" s="0">
-        <v>57</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13">
@@ -549,22 +549,22 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G13" s="0">
-        <v>176</v>
+        <v>269</v>
       </c>
       <c r="H13" s="0">
-        <v>116.3119104</v>
+        <v>236.4909864</v>
       </c>
       <c r="I13" s="0">
-        <v>0.0019422957481607384</v>
+        <v>0.001952341701944027</v>
       </c>
       <c r="J13" s="0">
-        <v>-1.2999783357839103e-05</v>
+        <v>-3.0092198418340354e-05</v>
       </c>
       <c r="K13" s="0">
         <v>2</v>
       </c>
       <c r="L13" s="0">
-        <v>57</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14">
@@ -587,16 +587,16 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G14" s="0">
-        <v>150</v>
+        <v>209</v>
       </c>
       <c r="H14" s="0">
-        <v>27.7283103</v>
+        <v>10.7656706</v>
       </c>
       <c r="I14" s="0">
-        <v>0.0013907086057423079</v>
+        <v>6.3456254398186474e-05</v>
       </c>
       <c r="J14" s="0">
-        <v>1.9944768976384678e-05</v>
+        <v>7.0544782584561883e-07</v>
       </c>
       <c r="K14" s="0">
         <v>0</v>
@@ -625,16 +625,16 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G15" s="0">
-        <v>153</v>
+        <v>269</v>
       </c>
       <c r="H15" s="0">
-        <v>64.405401299999994</v>
+        <v>115.43549659999999</v>
       </c>
       <c r="I15" s="0">
-        <v>0.0013907086057423079</v>
+        <v>6.676530033189465e-05</v>
       </c>
       <c r="J15" s="0">
-        <v>2.0256190713535646e-05</v>
+        <v>5.1701806504116313e-07</v>
       </c>
       <c r="K15" s="0">
         <v>0</v>
@@ -663,22 +663,22 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G16" s="0">
-        <v>165</v>
+        <v>251</v>
       </c>
       <c r="H16" s="0">
-        <v>94.311742300000006</v>
+        <v>92.037570799999997</v>
       </c>
       <c r="I16" s="0">
-        <v>0.0011907021309742749</v>
+        <v>0.00020161746254965252</v>
       </c>
       <c r="J16" s="0">
-        <v>1.5755517712114045e-05</v>
+        <v>-2.3781491897126006e-05</v>
       </c>
       <c r="K16" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" s="0">
-        <v>0</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17">
@@ -701,22 +701,22 @@
         <v>0.94999999999999996</v>
       </c>
       <c r="G17" s="0">
-        <v>182</v>
+        <v>269</v>
       </c>
       <c r="H17" s="0">
-        <v>71.535492099999999</v>
+        <v>221.23340959999999</v>
       </c>
       <c r="I17" s="0">
-        <v>0.0023318558688201207</v>
+        <v>0.00078415626376182601</v>
       </c>
       <c r="J17" s="0">
-        <v>-7.3498151964727416e-05</v>
+        <v>-3.0608607912803039e-05</v>
       </c>
       <c r="K17" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L17" s="0">
-        <v>30</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Yeah, it all works now. The system is defined using the size and the velocities of a Turtlebot and all the setups works.
</commit_message>
<xml_diff>
--- a/src/output/opt/all/data.xlsx
+++ b/src/output/opt/all/data.xlsx
@@ -96,7 +96,7 @@
         <v>221</v>
       </c>
       <c r="H1" s="0">
-        <v>26.866167099999998</v>
+        <v>25.860997000000001</v>
       </c>
       <c r="I1" s="0">
         <v>6.1648708908013106e-05</v>
@@ -134,7 +134,7 @@
         <v>269</v>
       </c>
       <c r="H2" s="0">
-        <v>73.478886000000003</v>
+        <v>71.420990399999994</v>
       </c>
       <c r="I2" s="0">
         <v>6.5519894709487048e-05</v>
@@ -172,7 +172,7 @@
         <v>269</v>
       </c>
       <c r="H3" s="0">
-        <v>82.138268400000001</v>
+        <v>80.4113507</v>
       </c>
       <c r="I3" s="0">
         <v>6.676530033189465e-05</v>
@@ -210,7 +210,7 @@
         <v>275</v>
       </c>
       <c r="H4" s="0">
-        <v>143.17481069999999</v>
+        <v>148.271277</v>
       </c>
       <c r="I4" s="0">
         <v>6.0603882801713027e-05</v>
@@ -248,7 +248,7 @@
         <v>238</v>
       </c>
       <c r="H5" s="0">
-        <v>79.355134800000002</v>
+        <v>77.787005300000004</v>
       </c>
       <c r="I5" s="0">
         <v>6.7715886985730833e-05</v>
@@ -286,7 +286,7 @@
         <v>779</v>
       </c>
       <c r="H6" s="0">
-        <v>404.45322729999998</v>
+        <v>318.72573240000003</v>
       </c>
       <c r="I6" s="0">
         <v>6.5152039799398764e-05</v>
@@ -324,7 +324,7 @@
         <v>1262</v>
       </c>
       <c r="H7" s="0">
-        <v>280.97373010000001</v>
+        <v>348.08444429999997</v>
       </c>
       <c r="I7" s="0">
         <v>0.00015597136462863759</v>
@@ -362,7 +362,7 @@
         <v>285</v>
       </c>
       <c r="H8" s="0">
-        <v>87.028548000000001</v>
+        <v>81.882517500000006</v>
       </c>
       <c r="I8" s="0">
         <v>6.7987289118054406e-05</v>
@@ -400,7 +400,7 @@
         <v>312</v>
       </c>
       <c r="H9" s="0">
-        <v>94.783641700000004</v>
+        <v>89.736347600000002</v>
       </c>
       <c r="I9" s="0">
         <v>6.8116042360788498e-05</v>
@@ -438,7 +438,7 @@
         <v>369</v>
       </c>
       <c r="H10" s="0">
-        <v>176.25475739999999</v>
+        <v>199.23783420000001</v>
       </c>
       <c r="I10" s="0">
         <v>0.00018531213506078892</v>
@@ -476,7 +476,7 @@
         <v>269</v>
       </c>
       <c r="H11" s="0">
-        <v>161.8426977</v>
+        <v>244.98417230000001</v>
       </c>
       <c r="I11" s="0">
         <v>0.00078415626376182601</v>
@@ -514,7 +514,7 @@
         <v>269</v>
       </c>
       <c r="H12" s="0">
-        <v>243.20405769999999</v>
+        <v>245.85245330000001</v>
       </c>
       <c r="I12" s="0">
         <v>0.00035683199620062389</v>
@@ -552,7 +552,7 @@
         <v>269</v>
       </c>
       <c r="H13" s="0">
-        <v>236.4909864</v>
+        <v>256.17017679999998</v>
       </c>
       <c r="I13" s="0">
         <v>0.001952341701944027</v>
@@ -590,7 +590,7 @@
         <v>209</v>
       </c>
       <c r="H14" s="0">
-        <v>10.7656706</v>
+        <v>10.634350400000001</v>
       </c>
       <c r="I14" s="0">
         <v>6.3456254398186474e-05</v>
@@ -628,7 +628,7 @@
         <v>269</v>
       </c>
       <c r="H15" s="0">
-        <v>115.43549659999999</v>
+        <v>110.98351220000001</v>
       </c>
       <c r="I15" s="0">
         <v>6.676530033189465e-05</v>
@@ -666,7 +666,7 @@
         <v>251</v>
       </c>
       <c r="H16" s="0">
-        <v>92.037570799999997</v>
+        <v>89.6249349</v>
       </c>
       <c r="I16" s="0">
         <v>0.00020161746254965252</v>
@@ -704,7 +704,7 @@
         <v>269</v>
       </c>
       <c r="H17" s="0">
-        <v>221.23340959999999</v>
+        <v>249.88699460000001</v>
       </c>
       <c r="I17" s="0">
         <v>0.00078415626376182601</v>

</xml_diff>

<commit_message>
- Tested all environmwnts in ideal case.
</commit_message>
<xml_diff>
--- a/src/output/opt/all/data.xlsx
+++ b/src/output/opt/all/data.xlsx
@@ -53,24 +53,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="true"/>
-    <col min="2" max="2" width="5.140625" customWidth="true"/>
-    <col min="3" max="3" width="2.140625" customWidth="true"/>
-    <col min="4" max="4" width="3.7109375" customWidth="true"/>
-    <col min="5" max="5" width="4.140625" customWidth="true"/>
-    <col min="6" max="6" width="4.7109375" customWidth="true"/>
-    <col min="7" max="7" width="5.140625" customWidth="true"/>
-    <col min="8" max="8" width="11.7109375" customWidth="true"/>
-    <col min="9" max="9" width="15.7109375" customWidth="true"/>
-    <col min="10" max="10" width="16.28515625" customWidth="true"/>
-    <col min="11" max="11" width="2.140625" customWidth="true"/>
-    <col min="12" max="12" width="4.140625" customWidth="true"/>
+    <col min="1" max="1" width="3" customWidth="true"/>
+    <col min="2" max="2" width="5" customWidth="true"/>
+    <col min="3" max="3" width="2" customWidth="true"/>
+    <col min="4" max="4" width="3.5546875" customWidth="true"/>
+    <col min="5" max="5" width="3" customWidth="true"/>
+    <col min="6" max="6" width="5" customWidth="true"/>
+    <col min="7" max="7" width="3.5546875" customWidth="true"/>
+    <col min="8" max="8" width="3" customWidth="true"/>
+    <col min="9" max="9" width="5" customWidth="true"/>
+    <col min="10" max="10" width="11.5546875" customWidth="true"/>
+    <col min="11" max="11" width="15.5546875" customWidth="true"/>
+    <col min="12" max="12" width="15.88671875" customWidth="true"/>
+    <col min="13" max="13" width="2" customWidth="true"/>
+    <col min="14" max="14" width="4" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -87,27 +89,33 @@
         <v>2.5</v>
       </c>
       <c r="E1" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F1" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G1" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H1" s="0">
+        <v>10</v>
+      </c>
+      <c r="I1" s="0">
         <v>221</v>
       </c>
-      <c r="H1" s="0">
-        <v>25.860997000000001</v>
-      </c>
-      <c r="I1" s="0">
-        <v>6.1648708908013106e-05</v>
-      </c>
       <c r="J1" s="0">
-        <v>7.6485959938137463e-07</v>
+        <v>37.592995899999998</v>
       </c>
       <c r="K1" s="0">
-        <v>0</v>
+        <v>6.4932694991970408e-06</v>
       </c>
       <c r="L1" s="0">
+        <v>8.0009670018521097e-08</v>
+      </c>
+      <c r="M1" s="0">
+        <v>0</v>
+      </c>
+      <c r="N1" s="0">
         <v>0</v>
       </c>
     </row>
@@ -125,27 +133,33 @@
         <v>2.5</v>
       </c>
       <c r="E2" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G2" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H2" s="0">
+        <v>10</v>
+      </c>
+      <c r="I2" s="0">
         <v>269</v>
       </c>
-      <c r="H2" s="0">
-        <v>71.420990399999994</v>
-      </c>
-      <c r="I2" s="0">
-        <v>6.5519894709487048e-05</v>
-      </c>
       <c r="J2" s="0">
-        <v>5.0572873784854949e-07</v>
+        <v>93.003292599999995</v>
       </c>
       <c r="K2" s="0">
-        <v>0</v>
+        <v>7.2171191389802658e-06</v>
       </c>
       <c r="L2" s="0">
+        <v>6.287673443285553e-08</v>
+      </c>
+      <c r="M2" s="0">
+        <v>0</v>
+      </c>
+      <c r="N2" s="0">
         <v>0</v>
       </c>
     </row>
@@ -163,27 +177,33 @@
         <v>2.5</v>
       </c>
       <c r="E3" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F3" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G3" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H3" s="0">
+        <v>10</v>
+      </c>
+      <c r="I3" s="0">
         <v>269</v>
       </c>
-      <c r="H3" s="0">
-        <v>80.4113507</v>
-      </c>
-      <c r="I3" s="0">
-        <v>6.676530033189465e-05</v>
-      </c>
       <c r="J3" s="0">
-        <v>5.1701806504116313e-07</v>
+        <v>100.07330109999999</v>
       </c>
       <c r="K3" s="0">
-        <v>0</v>
+        <v>7.1573757296494733e-06</v>
       </c>
       <c r="L3" s="0">
+        <v>5.8150525727170281e-08</v>
+      </c>
+      <c r="M3" s="0">
+        <v>0</v>
+      </c>
+      <c r="N3" s="0">
         <v>0</v>
       </c>
     </row>
@@ -201,27 +221,33 @@
         <v>2.5</v>
       </c>
       <c r="E4" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F4" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G4" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H4" s="0">
+        <v>10</v>
+      </c>
+      <c r="I4" s="0">
         <v>275</v>
       </c>
-      <c r="H4" s="0">
-        <v>148.271277</v>
-      </c>
-      <c r="I4" s="0">
-        <v>6.0603882801713027e-05</v>
-      </c>
       <c r="J4" s="0">
-        <v>6.556261854759074e-07</v>
+        <v>130.79598559999999</v>
       </c>
       <c r="K4" s="0">
-        <v>0</v>
+        <v>6.4342353602864222e-06</v>
       </c>
       <c r="L4" s="0">
+        <v>8.4126528430352524e-08</v>
+      </c>
+      <c r="M4" s="0">
+        <v>0</v>
+      </c>
+      <c r="N4" s="0">
         <v>0</v>
       </c>
     </row>
@@ -239,27 +265,33 @@
         <v>2.5</v>
       </c>
       <c r="E5" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F5" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G5" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H5" s="0">
+        <v>10</v>
+      </c>
+      <c r="I5" s="0">
         <v>238</v>
       </c>
-      <c r="H5" s="0">
-        <v>77.787005300000004</v>
-      </c>
-      <c r="I5" s="0">
-        <v>6.7715886985730833e-05</v>
-      </c>
       <c r="J5" s="0">
-        <v>6.1785031100708851e-07</v>
+        <v>100.3150967</v>
       </c>
       <c r="K5" s="0">
+        <v>7.2719002239818309e-06</v>
+      </c>
+      <c r="L5" s="0">
+        <v>3.4547054183295656e-08</v>
+      </c>
+      <c r="M5" s="0">
         <v>1</v>
       </c>
-      <c r="L5" s="0">
+      <c r="N5" s="0">
         <v>57</v>
       </c>
     </row>
@@ -277,27 +309,33 @@
         <v>2.5</v>
       </c>
       <c r="E6" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F6" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G6" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H6" s="0">
+        <v>10</v>
+      </c>
+      <c r="I6" s="0">
         <v>779</v>
       </c>
-      <c r="H6" s="0">
-        <v>318.72573240000003</v>
-      </c>
-      <c r="I6" s="0">
-        <v>6.5152039799398764e-05</v>
-      </c>
       <c r="J6" s="0">
-        <v>1.8010085309868908e-07</v>
+        <v>420.76224239999999</v>
       </c>
       <c r="K6" s="0">
-        <v>0</v>
+        <v>7.3346758511227961e-06</v>
       </c>
       <c r="L6" s="0">
+        <v>1.0632717650283736e-08</v>
+      </c>
+      <c r="M6" s="0">
+        <v>0</v>
+      </c>
+      <c r="N6" s="0">
         <v>0</v>
       </c>
     </row>
@@ -315,27 +353,33 @@
         <v>2.5</v>
       </c>
       <c r="E7" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F7" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G7" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H7" s="0">
+        <v>10</v>
+      </c>
+      <c r="I7" s="0">
         <v>1262</v>
       </c>
-      <c r="H7" s="0">
-        <v>348.08444429999997</v>
-      </c>
-      <c r="I7" s="0">
-        <v>0.00015597136462863759</v>
-      </c>
       <c r="J7" s="0">
-        <v>-1.6441482591255901e-06</v>
+        <v>436.4591729</v>
       </c>
       <c r="K7" s="0">
-        <v>0</v>
+        <v>1.7145014564734495e-05</v>
       </c>
       <c r="L7" s="0">
+        <v>-1.3758434871880631e-07</v>
+      </c>
+      <c r="M7" s="0">
+        <v>0</v>
+      </c>
+      <c r="N7" s="0">
         <v>0</v>
       </c>
     </row>
@@ -353,27 +397,33 @@
         <v>2.5</v>
       </c>
       <c r="E8" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F8" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G8" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H8" s="0">
+        <v>10</v>
+      </c>
+      <c r="I8" s="0">
         <v>285</v>
       </c>
-      <c r="H8" s="0">
-        <v>81.882517500000006</v>
-      </c>
-      <c r="I8" s="0">
-        <v>6.7987289118054406e-05</v>
-      </c>
       <c r="J8" s="0">
-        <v>4.3367886949577921e-07</v>
+        <v>108.8751674</v>
       </c>
       <c r="K8" s="0">
+        <v>7.287129319077934e-06</v>
+      </c>
+      <c r="L8" s="0">
+        <v>5.0733148107113003e-08</v>
+      </c>
+      <c r="M8" s="0">
         <v>1</v>
       </c>
-      <c r="L8" s="0">
+      <c r="N8" s="0">
         <v>61</v>
       </c>
     </row>
@@ -391,27 +441,33 @@
         <v>2.5</v>
       </c>
       <c r="E9" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F9" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G9" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H9" s="0">
+        <v>10</v>
+      </c>
+      <c r="I9" s="0">
         <v>312</v>
       </c>
-      <c r="H9" s="0">
-        <v>89.736347600000002</v>
-      </c>
-      <c r="I9" s="0">
-        <v>6.8116042360788498e-05</v>
-      </c>
       <c r="J9" s="0">
-        <v>6.0693372676457197e-07</v>
+        <v>119.39946329999999</v>
       </c>
       <c r="K9" s="0">
+        <v>2.7864391593190874e-05</v>
+      </c>
+      <c r="L9" s="0">
+        <v>3.6311749339572998e-08</v>
+      </c>
+      <c r="M9" s="0">
         <v>1</v>
       </c>
-      <c r="L9" s="0">
+      <c r="N9" s="0">
         <v>83</v>
       </c>
     </row>
@@ -429,27 +485,33 @@
         <v>2.5</v>
       </c>
       <c r="E10" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F10" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G10" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H10" s="0">
+        <v>10</v>
+      </c>
+      <c r="I10" s="0">
         <v>369</v>
       </c>
-      <c r="H10" s="0">
-        <v>199.23783420000001</v>
-      </c>
-      <c r="I10" s="0">
-        <v>0.00018531213506078892</v>
-      </c>
       <c r="J10" s="0">
-        <v>-4.3988692627432443e-06</v>
+        <v>228.01029969999999</v>
       </c>
       <c r="K10" s="0">
+        <v>2.7973201768949352e-05</v>
+      </c>
+      <c r="L10" s="0">
+        <v>-7.973671549211776e-07</v>
+      </c>
+      <c r="M10" s="0">
         <v>1</v>
       </c>
-      <c r="L10" s="0">
+      <c r="N10" s="0">
         <v>44</v>
       </c>
     </row>
@@ -467,27 +529,33 @@
         <v>2.5</v>
       </c>
       <c r="E11" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F11" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G11" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H11" s="0">
+        <v>10</v>
+      </c>
+      <c r="I11" s="0">
         <v>269</v>
       </c>
-      <c r="H11" s="0">
-        <v>244.98417230000001</v>
-      </c>
-      <c r="I11" s="0">
-        <v>0.00078415626376182601</v>
-      </c>
       <c r="J11" s="0">
-        <v>-3.0608607912803039e-05</v>
+        <v>231.72164889999999</v>
       </c>
       <c r="K11" s="0">
+        <v>7.5919017148429191e-05</v>
+      </c>
+      <c r="L11" s="0">
+        <v>-1.2505694785059221e-05</v>
+      </c>
+      <c r="M11" s="0">
         <v>2</v>
       </c>
-      <c r="L11" s="0">
+      <c r="N11" s="0">
         <v>172</v>
       </c>
     </row>
@@ -505,27 +573,33 @@
         <v>2.5</v>
       </c>
       <c r="E12" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F12" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G12" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H12" s="0">
+        <v>10</v>
+      </c>
+      <c r="I12" s="0">
         <v>269</v>
       </c>
-      <c r="H12" s="0">
-        <v>245.85245330000001</v>
-      </c>
-      <c r="I12" s="0">
-        <v>0.00035683199620062389</v>
-      </c>
       <c r="J12" s="0">
-        <v>-3.9766926691228031e-05</v>
+        <v>445.73144100000002</v>
       </c>
       <c r="K12" s="0">
+        <v>9.0414074238598374e-05</v>
+      </c>
+      <c r="L12" s="0">
+        <v>-2.2428847742544057e-05</v>
+      </c>
+      <c r="M12" s="0">
         <v>2</v>
       </c>
-      <c r="L12" s="0">
+      <c r="N12" s="0">
         <v>172</v>
       </c>
     </row>
@@ -543,28 +617,34 @@
         <v>2.5</v>
       </c>
       <c r="E13" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F13" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G13" s="0">
-        <v>269</v>
+        <v>0.90000000000000002</v>
       </c>
       <c r="H13" s="0">
-        <v>256.17017679999998</v>
+        <v>10</v>
       </c>
       <c r="I13" s="0">
-        <v>0.001952341701944027</v>
+        <v>270</v>
       </c>
       <c r="J13" s="0">
-        <v>-3.0092198418340354e-05</v>
+        <v>257.27560979999998</v>
       </c>
       <c r="K13" s="0">
+        <v>0.00015197332929051122</v>
+      </c>
+      <c r="L13" s="0">
+        <v>-1.3869979997114833e-05</v>
+      </c>
+      <c r="M13" s="0">
         <v>2</v>
       </c>
-      <c r="L13" s="0">
-        <v>172</v>
+      <c r="N13" s="0">
+        <v>173</v>
       </c>
     </row>
     <row r="14">
@@ -581,27 +661,33 @@
         <v>2.5</v>
       </c>
       <c r="E14" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F14" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G14" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H14" s="0">
+        <v>10</v>
+      </c>
+      <c r="I14" s="0">
         <v>209</v>
       </c>
-      <c r="H14" s="0">
-        <v>10.634350400000001</v>
-      </c>
-      <c r="I14" s="0">
-        <v>6.3456254398186474e-05</v>
-      </c>
       <c r="J14" s="0">
-        <v>7.0544782584561883e-07</v>
+        <v>16.840199900000002</v>
       </c>
       <c r="K14" s="0">
-        <v>0</v>
+        <v>6.8850238741369196e-06</v>
       </c>
       <c r="L14" s="0">
+        <v>5.7037244069216536e-08</v>
+      </c>
+      <c r="M14" s="0">
+        <v>0</v>
+      </c>
+      <c r="N14" s="0">
         <v>0</v>
       </c>
     </row>
@@ -619,27 +705,33 @@
         <v>2.5</v>
       </c>
       <c r="E15" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F15" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G15" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H15" s="0">
+        <v>10</v>
+      </c>
+      <c r="I15" s="0">
         <v>269</v>
       </c>
-      <c r="H15" s="0">
-        <v>110.98351220000001</v>
-      </c>
-      <c r="I15" s="0">
-        <v>6.676530033189465e-05</v>
-      </c>
       <c r="J15" s="0">
-        <v>5.1701806504116313e-07</v>
+        <v>123.6197784</v>
       </c>
       <c r="K15" s="0">
-        <v>0</v>
+        <v>7.1573757296494733e-06</v>
       </c>
       <c r="L15" s="0">
+        <v>5.8150525727170281e-08</v>
+      </c>
+      <c r="M15" s="0">
+        <v>0</v>
+      </c>
+      <c r="N15" s="0">
         <v>0</v>
       </c>
     </row>
@@ -657,27 +749,33 @@
         <v>2.5</v>
       </c>
       <c r="E16" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F16" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G16" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H16" s="0">
+        <v>10</v>
+      </c>
+      <c r="I16" s="0">
         <v>251</v>
       </c>
-      <c r="H16" s="0">
-        <v>89.6249349</v>
-      </c>
-      <c r="I16" s="0">
-        <v>0.00020161746254965252</v>
-      </c>
       <c r="J16" s="0">
-        <v>-2.3781491897126006e-05</v>
+        <v>120.6756374</v>
       </c>
       <c r="K16" s="0">
+        <v>9.4929486326389423e-05</v>
+      </c>
+      <c r="L16" s="0">
+        <v>-1.8186304555732276e-05</v>
+      </c>
+      <c r="M16" s="0">
         <v>1</v>
       </c>
-      <c r="L16" s="0">
+      <c r="N16" s="0">
         <v>83</v>
       </c>
     </row>
@@ -695,27 +793,33 @@
         <v>2.5</v>
       </c>
       <c r="E17" s="0">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F17" s="0">
-        <v>0.94999999999999996</v>
+        <v>1000</v>
       </c>
       <c r="G17" s="0">
+        <v>0.90000000000000002</v>
+      </c>
+      <c r="H17" s="0">
+        <v>10</v>
+      </c>
+      <c r="I17" s="0">
         <v>269</v>
       </c>
-      <c r="H17" s="0">
-        <v>249.88699460000001</v>
-      </c>
-      <c r="I17" s="0">
-        <v>0.00078415626376182601</v>
-      </c>
       <c r="J17" s="0">
-        <v>-3.0608607912803039e-05</v>
+        <v>243.72695870000001</v>
       </c>
       <c r="K17" s="0">
+        <v>7.5919017148429191e-05</v>
+      </c>
+      <c r="L17" s="0">
+        <v>-1.2505694785059221e-05</v>
+      </c>
+      <c r="M17" s="0">
         <v>2</v>
       </c>
-      <c r="L17" s="0">
+      <c r="N17" s="0">
         <v>172</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Generated all the base plot.
</commit_message>
<xml_diff>
--- a/src/output/opt/all/data.xlsx
+++ b/src/output/opt/all/data.xlsx
@@ -69,7 +69,7 @@
     <col min="8" max="8" width="3" customWidth="true"/>
     <col min="9" max="9" width="5" customWidth="true"/>
     <col min="10" max="10" width="11.5546875" customWidth="true"/>
-    <col min="11" max="11" width="15.5546875" customWidth="true"/>
+    <col min="11" max="11" width="15.21875" customWidth="true"/>
     <col min="12" max="12" width="15.88671875" customWidth="true"/>
     <col min="13" max="13" width="2" customWidth="true"/>
     <col min="14" max="14" width="4" customWidth="true"/>
@@ -104,7 +104,7 @@
         <v>221</v>
       </c>
       <c r="J1" s="0">
-        <v>37.592995899999998</v>
+        <v>46.355953999999997</v>
       </c>
       <c r="K1" s="0">
         <v>6.4932694991970408e-06</v>
@@ -148,7 +148,7 @@
         <v>269</v>
       </c>
       <c r="J2" s="0">
-        <v>93.003292599999995</v>
+        <v>112.85662689999999</v>
       </c>
       <c r="K2" s="0">
         <v>7.2171191389802658e-06</v>
@@ -192,7 +192,7 @@
         <v>269</v>
       </c>
       <c r="J3" s="0">
-        <v>100.07330109999999</v>
+        <v>118.6160898</v>
       </c>
       <c r="K3" s="0">
         <v>7.1573757296494733e-06</v>
@@ -236,7 +236,7 @@
         <v>275</v>
       </c>
       <c r="J4" s="0">
-        <v>130.79598559999999</v>
+        <v>154.50660579999999</v>
       </c>
       <c r="K4" s="0">
         <v>6.4342353602864222e-06</v>
@@ -280,7 +280,7 @@
         <v>238</v>
       </c>
       <c r="J5" s="0">
-        <v>100.3150967</v>
+        <v>107.7844659</v>
       </c>
       <c r="K5" s="0">
         <v>7.2719002239818309e-06</v>
@@ -324,7 +324,7 @@
         <v>779</v>
       </c>
       <c r="J6" s="0">
-        <v>420.76224239999999</v>
+        <v>438.61068760000001</v>
       </c>
       <c r="K6" s="0">
         <v>7.3346758511227961e-06</v>
@@ -365,16 +365,16 @@
         <v>10</v>
       </c>
       <c r="I7" s="0">
-        <v>1262</v>
+        <v>1270</v>
       </c>
       <c r="J7" s="0">
-        <v>436.4591729</v>
+        <v>560.41570300000001</v>
       </c>
       <c r="K7" s="0">
         <v>1.7145014564734495e-05</v>
       </c>
       <c r="L7" s="0">
-        <v>-1.3758434871880631e-07</v>
+        <v>-1.3667309257269633e-06</v>
       </c>
       <c r="M7" s="0">
         <v>0</v>
@@ -412,7 +412,7 @@
         <v>285</v>
       </c>
       <c r="J8" s="0">
-        <v>108.8751674</v>
+        <v>118.2736427</v>
       </c>
       <c r="K8" s="0">
         <v>7.287129319077934e-06</v>
@@ -456,7 +456,7 @@
         <v>312</v>
       </c>
       <c r="J9" s="0">
-        <v>119.39946329999999</v>
+        <v>131.3902247</v>
       </c>
       <c r="K9" s="0">
         <v>2.7864391593190874e-05</v>
@@ -500,7 +500,7 @@
         <v>369</v>
       </c>
       <c r="J10" s="0">
-        <v>228.01029969999999</v>
+        <v>199.83500549999999</v>
       </c>
       <c r="K10" s="0">
         <v>2.7973201768949352e-05</v>
@@ -544,7 +544,7 @@
         <v>269</v>
       </c>
       <c r="J11" s="0">
-        <v>231.72164889999999</v>
+        <v>200.7586077</v>
       </c>
       <c r="K11" s="0">
         <v>7.5919017148429191e-05</v>
@@ -588,7 +588,7 @@
         <v>269</v>
       </c>
       <c r="J12" s="0">
-        <v>445.73144100000002</v>
+        <v>432.87870320000002</v>
       </c>
       <c r="K12" s="0">
         <v>9.0414074238598374e-05</v>
@@ -632,7 +632,7 @@
         <v>270</v>
       </c>
       <c r="J13" s="0">
-        <v>257.27560979999998</v>
+        <v>227.20696989999999</v>
       </c>
       <c r="K13" s="0">
         <v>0.00015197332929051122</v>

</xml_diff>